<commit_message>
working on running electronic_only
</commit_message>
<xml_diff>
--- a/opv_results_v2.xlsx
+++ b/opv_results_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stanley Lo\Documents\Summer 2021 NSERC\ml_for_opvs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7762EB-66C4-4435-95DD-0BCE18970097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C61040-374A-4AD2-B22E-0D6DC05B9CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{B4BECBF8-D04C-4ADA-84A7-E985FD3B894C}"/>
+    <workbookView xWindow="38280" yWindow="1260" windowWidth="29040" windowHeight="15840" xr2:uid="{B4BECBF8-D04C-4ADA-84A7-E985FD3B894C}"/>
   </bookViews>
   <sheets>
     <sheet name="opv_results" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="33">
   <si>
     <t>Model</t>
   </si>
@@ -126,6 +126,15 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>JSC</t>
+  </si>
+  <si>
+    <t>VOC</t>
   </si>
 </sst>
 </file>
@@ -477,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66BCD09-9543-4563-A8CC-8F27C3F15D07}">
-  <dimension ref="A1:I166"/>
+  <dimension ref="A1:I181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="G84" sqref="G84"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="M77" sqref="L77:M77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2761,7 +2770,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>18</v>
       </c>
@@ -2775,7 +2784,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>18</v>
       </c>
@@ -2789,7 +2798,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>18</v>
       </c>
@@ -2803,7 +2812,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>18</v>
       </c>
@@ -2817,7 +2826,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>18</v>
       </c>
@@ -2831,7 +2840,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>18</v>
       </c>
@@ -2843,6 +2852,261 @@
       </c>
       <c r="D166" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>5</v>
+      </c>
+      <c r="B167" t="s">
+        <v>29</v>
+      </c>
+      <c r="C167" t="s">
+        <v>28</v>
+      </c>
+      <c r="D167" t="s">
+        <v>30</v>
+      </c>
+      <c r="E167">
+        <v>0.25258670773465902</v>
+      </c>
+      <c r="F167">
+        <v>3.7576020888399002E-2</v>
+      </c>
+      <c r="G167">
+        <v>0.121427776682782</v>
+      </c>
+      <c r="H167">
+        <v>1.6228970514301201E-2</v>
+      </c>
+      <c r="I167">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>15</v>
+      </c>
+      <c r="B168" t="s">
+        <v>29</v>
+      </c>
+      <c r="C168" t="s">
+        <v>28</v>
+      </c>
+      <c r="D168" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>16</v>
+      </c>
+      <c r="B169" t="s">
+        <v>29</v>
+      </c>
+      <c r="C169" t="s">
+        <v>28</v>
+      </c>
+      <c r="D169" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>17</v>
+      </c>
+      <c r="B170" t="s">
+        <v>29</v>
+      </c>
+      <c r="C170" t="s">
+        <v>28</v>
+      </c>
+      <c r="D170" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>18</v>
+      </c>
+      <c r="B171" t="s">
+        <v>29</v>
+      </c>
+      <c r="C171" t="s">
+        <v>28</v>
+      </c>
+      <c r="D171" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>5</v>
+      </c>
+      <c r="B172" t="s">
+        <v>29</v>
+      </c>
+      <c r="C172" t="s">
+        <v>28</v>
+      </c>
+      <c r="D172" t="s">
+        <v>31</v>
+      </c>
+      <c r="E172">
+        <v>0.65633543982259201</v>
+      </c>
+      <c r="F172">
+        <v>5.0932560971677303E-2</v>
+      </c>
+      <c r="G172">
+        <v>0.13704075275446201</v>
+      </c>
+      <c r="H172">
+        <v>7.4415413768480296E-3</v>
+      </c>
+      <c r="I172">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>15</v>
+      </c>
+      <c r="B173" t="s">
+        <v>29</v>
+      </c>
+      <c r="C173" t="s">
+        <v>28</v>
+      </c>
+      <c r="D173" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>16</v>
+      </c>
+      <c r="B174" t="s">
+        <v>29</v>
+      </c>
+      <c r="C174" t="s">
+        <v>28</v>
+      </c>
+      <c r="D174" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>17</v>
+      </c>
+      <c r="B175" t="s">
+        <v>29</v>
+      </c>
+      <c r="C175" t="s">
+        <v>28</v>
+      </c>
+      <c r="D175" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>18</v>
+      </c>
+      <c r="B176" t="s">
+        <v>29</v>
+      </c>
+      <c r="C176" t="s">
+        <v>28</v>
+      </c>
+      <c r="D176" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>5</v>
+      </c>
+      <c r="B177" t="s">
+        <v>29</v>
+      </c>
+      <c r="C177" t="s">
+        <v>28</v>
+      </c>
+      <c r="D177" t="s">
+        <v>32</v>
+      </c>
+      <c r="E177">
+        <v>0.66585182916198404</v>
+      </c>
+      <c r="F177">
+        <v>4.8133234329250499E-2</v>
+      </c>
+      <c r="G177">
+        <v>6.3665221036705799E-2</v>
+      </c>
+      <c r="H177">
+        <v>8.0769472002819205E-3</v>
+      </c>
+      <c r="I177">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>15</v>
+      </c>
+      <c r="B178" t="s">
+        <v>29</v>
+      </c>
+      <c r="C178" t="s">
+        <v>28</v>
+      </c>
+      <c r="D178" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>16</v>
+      </c>
+      <c r="B179" t="s">
+        <v>29</v>
+      </c>
+      <c r="C179" t="s">
+        <v>28</v>
+      </c>
+      <c r="D179" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>17</v>
+      </c>
+      <c r="B180" t="s">
+        <v>29</v>
+      </c>
+      <c r="C180" t="s">
+        <v>28</v>
+      </c>
+      <c r="D180" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>18</v>
+      </c>
+      <c r="B181" t="s">
+        <v>29</v>
+      </c>
+      <c r="C181" t="s">
+        <v>28</v>
+      </c>
+      <c r="D181" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed anomaly for postprocess data
</commit_message>
<xml_diff>
--- a/opv_results_v2.xlsx
+++ b/opv_results_v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stanley Lo\Documents\Summer 2021 NSERC\ml_for_opvs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stanley Lo\My Documents\Summer 2021 NSERC\ml_for_opvs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C61040-374A-4AD2-B22E-0D6DC05B9CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD5DEED-53BE-485A-BD48-CD5CF64767F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="1260" windowWidth="29040" windowHeight="15840" xr2:uid="{B4BECBF8-D04C-4ADA-84A7-E985FD3B894C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{B4BECBF8-D04C-4ADA-84A7-E985FD3B894C}"/>
   </bookViews>
   <sheets>
     <sheet name="opv_results" sheetId="1" r:id="rId1"/>
@@ -489,7 +489,7 @@
   <dimension ref="A1:I181"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="M77" sqref="L77:M77"/>
+      <selection activeCell="M78" sqref="M78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
working on running sklearn models
</commit_message>
<xml_diff>
--- a/opv_results_v2.xlsx
+++ b/opv_results_v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stanley Lo\My Documents\Summer 2021 NSERC\ml_for_opvs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stanley Lo\Documents\Summer 2021 NSERC\ml_for_opvs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD5DEED-53BE-485A-BD48-CD5CF64767F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F935216F-C7F5-43C9-9484-A45A5F93DCA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{B4BECBF8-D04C-4ADA-84A7-E985FD3B894C}"/>
+    <workbookView xWindow="-8820" yWindow="-516" windowWidth="18432" windowHeight="9768" xr2:uid="{B4BECBF8-D04C-4ADA-84A7-E985FD3B894C}"/>
   </bookViews>
   <sheets>
     <sheet name="opv_results" sheetId="1" r:id="rId1"/>
@@ -488,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66BCD09-9543-4563-A8CC-8F27C3F15D07}">
   <dimension ref="A1:I181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="M78" sqref="M78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,19 +514,19 @@
         <v>26</v>
       </c>
       <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
         <v>19</v>
-      </c>
-      <c r="F1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -542,6 +542,21 @@
       <c r="D2" t="s">
         <v>27</v>
       </c>
+      <c r="E2">
+        <v>0.62813610018402299</v>
+      </c>
+      <c r="F2">
+        <v>7.2833427240581297E-2</v>
+      </c>
+      <c r="G2">
+        <v>0.157762285934057</v>
+      </c>
+      <c r="H2">
+        <v>2.4092237265460802E-2</v>
+      </c>
+      <c r="I2">
+        <v>556</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -556,6 +571,21 @@
       <c r="D3" t="s">
         <v>27</v>
       </c>
+      <c r="E3">
+        <v>0.63877089008832999</v>
+      </c>
+      <c r="F3">
+        <v>7.9113294455477698E-2</v>
+      </c>
+      <c r="G3">
+        <v>0.156107845269398</v>
+      </c>
+      <c r="H3">
+        <v>2.55185545309627E-2</v>
+      </c>
+      <c r="I3">
+        <v>556</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -570,6 +600,21 @@
       <c r="D4" t="s">
         <v>27</v>
       </c>
+      <c r="E4">
+        <v>0.64649318977724501</v>
+      </c>
+      <c r="F4">
+        <v>6.0121236629882301E-2</v>
+      </c>
+      <c r="G4">
+        <v>0.154401391889916</v>
+      </c>
+      <c r="H4">
+        <v>2.3177355135618399E-2</v>
+      </c>
+      <c r="I4">
+        <v>556</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -584,6 +629,21 @@
       <c r="D5" t="s">
         <v>27</v>
       </c>
+      <c r="E5">
+        <v>0.49359585421651297</v>
+      </c>
+      <c r="F5">
+        <v>7.37843769701262E-2</v>
+      </c>
+      <c r="G5">
+        <v>0.176627652838907</v>
+      </c>
+      <c r="H5">
+        <v>2.2985116466043499E-2</v>
+      </c>
+      <c r="I5">
+        <v>556</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -598,6 +658,21 @@
       <c r="D6" t="s">
         <v>27</v>
       </c>
+      <c r="E6">
+        <v>0.68288723323085099</v>
+      </c>
+      <c r="F6">
+        <v>6.7555834775905793E-2</v>
+      </c>
+      <c r="G6">
+        <v>0.14637437701699699</v>
+      </c>
+      <c r="H6">
+        <v>1.9779066086000101E-2</v>
+      </c>
+      <c r="I6">
+        <v>556</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -612,6 +687,21 @@
       <c r="D7" t="s">
         <v>27</v>
       </c>
+      <c r="E7">
+        <v>0.675303582386243</v>
+      </c>
+      <c r="F7">
+        <v>4.8045653484017799E-2</v>
+      </c>
+      <c r="G7">
+        <v>0.14817191299363999</v>
+      </c>
+      <c r="H7">
+        <v>1.3441455174449699E-2</v>
+      </c>
+      <c r="I7">
+        <v>556</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -626,6 +716,21 @@
       <c r="D8" t="s">
         <v>27</v>
       </c>
+      <c r="E8">
+        <v>0.65101278918567995</v>
+      </c>
+      <c r="F8">
+        <v>5.6228455623029E-2</v>
+      </c>
+      <c r="G8">
+        <v>0.153485315711967</v>
+      </c>
+      <c r="H8">
+        <v>1.9843083811824199E-2</v>
+      </c>
+      <c r="I8">
+        <v>556</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -640,6 +745,21 @@
       <c r="D9" t="s">
         <v>27</v>
       </c>
+      <c r="E9">
+        <v>0.72698273872294505</v>
+      </c>
+      <c r="F9">
+        <v>5.5640040279394003E-2</v>
+      </c>
+      <c r="G9">
+        <v>0.13842668840805999</v>
+      </c>
+      <c r="H9">
+        <v>1.6471351077796299E-2</v>
+      </c>
+      <c r="I9">
+        <v>556</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -1691,6 +1811,21 @@
       <c r="D83" t="s">
         <v>27</v>
       </c>
+      <c r="E83">
+        <v>0.55302783911153297</v>
+      </c>
+      <c r="F83">
+        <v>3.0489556892871798E-2</v>
+      </c>
+      <c r="G83">
+        <v>0.16844429999999999</v>
+      </c>
+      <c r="H83">
+        <v>1.2271737E-2</v>
+      </c>
+      <c r="I83">
+        <v>447</v>
+      </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
@@ -1704,6 +1839,21 @@
       </c>
       <c r="D84" t="s">
         <v>27</v>
+      </c>
+      <c r="E84">
+        <v>0.54921497712617395</v>
+      </c>
+      <c r="F84">
+        <v>3.5687978617597801E-2</v>
+      </c>
+      <c r="G84">
+        <v>0.16964984164206001</v>
+      </c>
+      <c r="H84">
+        <v>1.35076548325601E-2</v>
+      </c>
+      <c r="I84">
+        <v>447</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
start working on DL pipeline
</commit_message>
<xml_diff>
--- a/opv_results_v2.xlsx
+++ b/opv_results_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stanley Lo\Documents\Summer 2021 NSERC\ml_for_opvs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F935216F-C7F5-43C9-9484-A45A5F93DCA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D9645A-BC47-48DF-9E61-404276A610DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8820" yWindow="-516" windowWidth="18432" windowHeight="9768" xr2:uid="{B4BECBF8-D04C-4ADA-84A7-E985FD3B894C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{B4BECBF8-D04C-4ADA-84A7-E985FD3B894C}"/>
   </bookViews>
   <sheets>
     <sheet name="opv_results" sheetId="1" r:id="rId1"/>
@@ -489,7 +489,7 @@
   <dimension ref="A1:I181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -774,6 +774,21 @@
       <c r="D10" t="s">
         <v>27</v>
       </c>
+      <c r="E10">
+        <v>0.61635443823195002</v>
+      </c>
+      <c r="F10">
+        <v>7.1095427005393896E-2</v>
+      </c>
+      <c r="G10">
+        <v>0.16054202616214699</v>
+      </c>
+      <c r="H10">
+        <v>2.4363607168197601E-2</v>
+      </c>
+      <c r="I10">
+        <v>556</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -788,6 +803,21 @@
       <c r="D11" t="s">
         <v>27</v>
       </c>
+      <c r="E11">
+        <v>0.62607187578574197</v>
+      </c>
+      <c r="F11">
+        <v>8.0043212497972194E-2</v>
+      </c>
+      <c r="G11">
+        <v>0.15966604650020599</v>
+      </c>
+      <c r="H11">
+        <v>2.56536491215229E-2</v>
+      </c>
+      <c r="I11">
+        <v>556</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -802,6 +832,21 @@
       <c r="D12" t="s">
         <v>27</v>
       </c>
+      <c r="E12">
+        <v>0.63635914334342403</v>
+      </c>
+      <c r="F12">
+        <v>6.5593093645026704E-2</v>
+      </c>
+      <c r="G12">
+        <v>0.156994849443435</v>
+      </c>
+      <c r="H12">
+        <v>2.34825499355793E-2</v>
+      </c>
+      <c r="I12">
+        <v>556</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -816,6 +861,21 @@
       <c r="D13" t="s">
         <v>27</v>
       </c>
+      <c r="E13">
+        <v>0.49433722894073201</v>
+      </c>
+      <c r="F13">
+        <v>7.7384885219848307E-2</v>
+      </c>
+      <c r="G13">
+        <v>0.176036447286605</v>
+      </c>
+      <c r="H13">
+        <v>2.41741314530372E-2</v>
+      </c>
+      <c r="I13">
+        <v>556</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -830,6 +890,21 @@
       <c r="D14" t="s">
         <v>27</v>
       </c>
+      <c r="E14">
+        <v>0.68772552132417297</v>
+      </c>
+      <c r="F14">
+        <v>8.1548127360052694E-2</v>
+      </c>
+      <c r="G14">
+        <v>0.14705356955528201</v>
+      </c>
+      <c r="H14">
+        <v>2.1178727969527199E-2</v>
+      </c>
+      <c r="I14">
+        <v>556</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -844,6 +919,21 @@
       <c r="D15" t="s">
         <v>27</v>
       </c>
+      <c r="E15">
+        <v>0.67575033016347297</v>
+      </c>
+      <c r="F15">
+        <v>7.3512473110954907E-2</v>
+      </c>
+      <c r="G15">
+        <v>0.148529052734375</v>
+      </c>
+      <c r="H15">
+        <v>1.48715740069746E-2</v>
+      </c>
+      <c r="I15">
+        <v>556</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -858,8 +948,23 @@
       <c r="D16" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>0.652411369232893</v>
+      </c>
+      <c r="F16">
+        <v>7.5018817297932902E-2</v>
+      </c>
+      <c r="G16">
+        <v>0.154740735888481</v>
+      </c>
+      <c r="H16">
+        <v>2.17382330447435E-2</v>
+      </c>
+      <c r="I16">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -872,8 +977,23 @@
       <c r="D17" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>0.71993180364388798</v>
+      </c>
+      <c r="F17">
+        <v>6.6144075928657203E-2</v>
+      </c>
+      <c r="G17">
+        <v>0.139440968632698</v>
+      </c>
+      <c r="H17">
+        <v>1.83883681893348E-2</v>
+      </c>
+      <c r="I17">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -887,7 +1007,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -901,7 +1021,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -915,7 +1035,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -929,7 +1049,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -943,7 +1063,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -957,7 +1077,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -971,7 +1091,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -985,7 +1105,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -999,7 +1119,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -1013,7 +1133,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -1027,7 +1147,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -1041,7 +1161,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -1055,7 +1175,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -1069,7 +1189,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -1083,7 +1203,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -1097,7 +1217,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>18</v>
       </c>
@@ -1111,7 +1231,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -1125,7 +1245,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>18</v>
       </c>
@@ -1139,7 +1259,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>18</v>
       </c>
@@ -1153,7 +1273,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>18</v>
       </c>
@@ -1167,7 +1287,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>18</v>
       </c>
@@ -1181,7 +1301,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -1195,7 +1315,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>18</v>
       </c>
@@ -1209,7 +1329,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>5</v>
       </c>
@@ -1222,8 +1342,23 @@
       <c r="D42" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E42">
+        <v>0.63911453853812805</v>
+      </c>
+      <c r="F42">
+        <v>3.2522503023203503E-2</v>
+      </c>
+      <c r="G42">
+        <v>0.15611515512705701</v>
+      </c>
+      <c r="H42">
+        <v>1.21339535146861E-2</v>
+      </c>
+      <c r="I42">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -1236,8 +1371,23 @@
       <c r="D43" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E43">
+        <v>0.65682806789106596</v>
+      </c>
+      <c r="F43">
+        <v>2.9563898247692299E-2</v>
+      </c>
+      <c r="G43">
+        <v>0.15352006748400501</v>
+      </c>
+      <c r="H43">
+        <v>1.16529925882198E-2</v>
+      </c>
+      <c r="I43">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -1250,8 +1400,23 @@
       <c r="D44" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E44">
+        <v>0.651121451979078</v>
+      </c>
+      <c r="F44">
+        <v>1.5348962892391E-2</v>
+      </c>
+      <c r="G44">
+        <v>0.153760794688625</v>
+      </c>
+      <c r="H44">
+        <v>9.6016212375992799E-3</v>
+      </c>
+      <c r="I44">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>5</v>
       </c>
@@ -1264,8 +1429,23 @@
       <c r="D45" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E45">
+        <v>0.56312415504781199</v>
+      </c>
+      <c r="F45">
+        <v>3.8914309861472297E-2</v>
+      </c>
+      <c r="G45">
+        <v>0.17100185075917501</v>
+      </c>
+      <c r="H45">
+        <v>1.07003483878228E-2</v>
+      </c>
+      <c r="I45">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>5</v>
       </c>
@@ -1278,8 +1458,23 @@
       <c r="D46" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E46">
+        <v>0.69665226596533603</v>
+      </c>
+      <c r="F46">
+        <v>2.24192081331595E-2</v>
+      </c>
+      <c r="G46">
+        <v>0.14508134475361101</v>
+      </c>
+      <c r="H46">
+        <v>1.0029892229590999E-2</v>
+      </c>
+      <c r="I46">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -1292,8 +1487,23 @@
       <c r="D47" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E47">
+        <v>0.695116116823148</v>
+      </c>
+      <c r="F47">
+        <v>1.3071220611402101E-2</v>
+      </c>
+      <c r="G47">
+        <v>0.145537560342584</v>
+      </c>
+      <c r="H47">
+        <v>9.7381610904078205E-3</v>
+      </c>
+      <c r="I47">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>5</v>
       </c>
@@ -1306,8 +1516,23 @@
       <c r="D48" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E48">
+        <v>0.58590629073124401</v>
+      </c>
+      <c r="F48">
+        <v>5.6501301209272298E-2</v>
+      </c>
+      <c r="G48">
+        <v>0.16881166342197401</v>
+      </c>
+      <c r="H48">
+        <v>1.5218371091253799E-2</v>
+      </c>
+      <c r="I48">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -1320,8 +1545,23 @@
       <c r="D49" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E49">
+        <v>0.74228318921537395</v>
+      </c>
+      <c r="F49">
+        <v>1.9902063646396101E-2</v>
+      </c>
+      <c r="G49">
+        <v>0.13650432155313699</v>
+      </c>
+      <c r="H49">
+        <v>1.0602340360635501E-2</v>
+      </c>
+      <c r="I49">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>15</v>
       </c>
@@ -1335,7 +1575,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -1349,7 +1589,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>15</v>
       </c>
@@ -1363,7 +1603,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>15</v>
       </c>
@@ -1377,7 +1617,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>15</v>
       </c>
@@ -1391,7 +1631,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>15</v>
       </c>
@@ -1405,7 +1645,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>15</v>
       </c>
@@ -1419,7 +1659,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>15</v>
       </c>
@@ -1433,7 +1673,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>16</v>
       </c>
@@ -1447,7 +1687,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>16</v>
       </c>
@@ -1461,7 +1701,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>16</v>
       </c>
@@ -1475,7 +1715,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>16</v>
       </c>
@@ -1489,7 +1729,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>16</v>
       </c>
@@ -1503,7 +1743,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>16</v>
       </c>
@@ -1517,7 +1757,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
working on running models and visualization
</commit_message>
<xml_diff>
--- a/opv_results_v2.xlsx
+++ b/opv_results_v2.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stanley Lo\My Documents\Summer 2021 NSERC\ml_for_opvs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89633851-F23E-47EF-947D-0254AB8AE1AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB57043-7C17-48CA-B6BF-F9820DA0148F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="1260" windowWidth="29040" windowHeight="15840" xr2:uid="{B4BECBF8-D04C-4ADA-84A7-E985FD3B894C}"/>
   </bookViews>
   <sheets>
     <sheet name="opv_results" sheetId="1" r:id="rId1"/>
-    <sheet name="legend" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="32">
   <si>
     <t>Model</t>
   </si>
@@ -102,9 +101,6 @@
   </si>
   <si>
     <t>"device"</t>
-  </si>
-  <si>
-    <t>Legend</t>
   </si>
   <si>
     <t>R_mean</t>
@@ -486,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66BCD09-9543-4563-A8CC-8F27C3F15D07}">
-  <dimension ref="A1:I181"/>
+  <dimension ref="A1:I237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="K175" sqref="K175"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,16 +507,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
@@ -540,7 +536,22 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="E2">
+        <v>0.626848451617387</v>
+      </c>
+      <c r="F2">
+        <v>6.0966533086275899E-2</v>
+      </c>
+      <c r="G2">
+        <v>2.4217868695645399</v>
+      </c>
+      <c r="H2">
+        <v>0.106092388782347</v>
+      </c>
+      <c r="I2">
+        <v>555</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -554,7 +565,22 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="E3">
+        <v>0.63290453708485395</v>
+      </c>
+      <c r="F3">
+        <v>5.97901010074956E-2</v>
+      </c>
+      <c r="G3">
+        <v>2.4088991180302601</v>
+      </c>
+      <c r="H3">
+        <v>0.10830024316331099</v>
+      </c>
+      <c r="I3">
+        <v>555</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -568,7 +594,22 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="E4">
+        <v>0.62007024356324403</v>
+      </c>
+      <c r="F4">
+        <v>7.3907164879719101E-2</v>
+      </c>
+      <c r="G4">
+        <v>2.4317486685441798</v>
+      </c>
+      <c r="H4">
+        <v>0.14147431851246001</v>
+      </c>
+      <c r="I4">
+        <v>555</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -582,7 +623,22 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="E5">
+        <v>0.50665286290468203</v>
+      </c>
+      <c r="F5">
+        <v>0.102629365161089</v>
+      </c>
+      <c r="G5">
+        <v>2.6837097856350201</v>
+      </c>
+      <c r="H5">
+        <v>0.151553599918022</v>
+      </c>
+      <c r="I5">
+        <v>555</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -596,7 +652,22 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="E6">
+        <v>0.66926575938451105</v>
+      </c>
+      <c r="F6">
+        <v>4.6897399331156497E-2</v>
+      </c>
+      <c r="G6">
+        <v>2.3111136639701702</v>
+      </c>
+      <c r="H6">
+        <v>8.2958599105666997E-2</v>
+      </c>
+      <c r="I6">
+        <v>555</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -610,7 +681,22 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="E7">
+        <v>0.65686928972982195</v>
+      </c>
+      <c r="F7">
+        <v>8.4044871573515798E-2</v>
+      </c>
+      <c r="G7">
+        <v>2.3192449474358998</v>
+      </c>
+      <c r="H7">
+        <v>0.198496678380082</v>
+      </c>
+      <c r="I7">
+        <v>555</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -624,7 +710,22 @@
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="E8">
+        <v>0.64063766584206305</v>
+      </c>
+      <c r="F8">
+        <v>7.9157763288474597E-2</v>
+      </c>
+      <c r="G8">
+        <v>2.4185266336346798</v>
+      </c>
+      <c r="H8">
+        <v>0.22174422385654899</v>
+      </c>
+      <c r="I8">
+        <v>555</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -638,12 +739,27 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="E9">
+        <v>0.71767510090911701</v>
+      </c>
+      <c r="F9">
+        <v>5.44419668745737E-2</v>
+      </c>
+      <c r="G9">
+        <v>2.1470942126205101</v>
+      </c>
+      <c r="H9">
+        <v>0.17362982698853899</v>
+      </c>
+      <c r="I9">
+        <v>555</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -652,12 +768,27 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="E10">
+        <v>0.43889927552008801</v>
+      </c>
+      <c r="F10">
+        <v>0.111639393524015</v>
+      </c>
+      <c r="G10">
+        <v>9.2160741575172604</v>
+      </c>
+      <c r="H10">
+        <v>1.32538909970439</v>
+      </c>
+      <c r="I10">
+        <v>555</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -666,12 +797,27 @@
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="E11">
+        <v>0.43129819481319898</v>
+      </c>
+      <c r="F11">
+        <v>0.110365592880441</v>
+      </c>
+      <c r="G11">
+        <v>9.2417551131216698</v>
+      </c>
+      <c r="H11">
+        <v>1.2971573979209099</v>
+      </c>
+      <c r="I11">
+        <v>555</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
@@ -680,12 +826,27 @@
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="E12">
+        <v>0.45566467780923797</v>
+      </c>
+      <c r="F12">
+        <v>0.12534346398377499</v>
+      </c>
+      <c r="G12">
+        <v>9.1079019213248795</v>
+      </c>
+      <c r="H12">
+        <v>1.30773663141059</v>
+      </c>
+      <c r="I12">
+        <v>555</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -694,12 +855,27 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="E13">
+        <v>0.33176925491676601</v>
+      </c>
+      <c r="F13">
+        <v>0.180305373657526</v>
+      </c>
+      <c r="G13">
+        <v>9.5937077757615707</v>
+      </c>
+      <c r="H13">
+        <v>1.23224926505007</v>
+      </c>
+      <c r="I13">
+        <v>555</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
@@ -708,12 +884,27 @@
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="E14">
+        <v>0.52157447633682896</v>
+      </c>
+      <c r="F14">
+        <v>0.124080774279688</v>
+      </c>
+      <c r="G14">
+        <v>8.76747937964074</v>
+      </c>
+      <c r="H14">
+        <v>0.90903024530300103</v>
+      </c>
+      <c r="I14">
+        <v>555</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
@@ -722,12 +913,27 @@
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="E15">
+        <v>0.56293143692342695</v>
+      </c>
+      <c r="F15">
+        <v>0.10580193484214601</v>
+      </c>
+      <c r="G15">
+        <v>8.3708614943632593</v>
+      </c>
+      <c r="H15">
+        <v>1.1475233314194</v>
+      </c>
+      <c r="I15">
+        <v>555</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
         <v>13</v>
@@ -736,12 +942,27 @@
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="E16">
+        <v>0.52921696391373896</v>
+      </c>
+      <c r="F16">
+        <v>0.12760765491484799</v>
+      </c>
+      <c r="G16">
+        <v>8.6663812863826006</v>
+      </c>
+      <c r="H16">
+        <v>1.22941026313955</v>
+      </c>
+      <c r="I16">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B17" t="s">
         <v>14</v>
@@ -750,12 +971,27 @@
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="E17">
+        <v>0.59810205992542997</v>
+      </c>
+      <c r="F17">
+        <v>0.10473825420121501</v>
+      </c>
+      <c r="G17">
+        <v>8.0812044805949306</v>
+      </c>
+      <c r="H17">
+        <v>1.14858414292184</v>
+      </c>
+      <c r="I17">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -764,12 +1000,27 @@
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="E18">
+        <v>0.44351695442285</v>
+      </c>
+      <c r="F18">
+        <v>4.0416238261610102E-2</v>
+      </c>
+      <c r="G18">
+        <v>0.16163152849635501</v>
+      </c>
+      <c r="H18">
+        <v>8.5088016608031395E-3</v>
+      </c>
+      <c r="I18">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -778,12 +1029,27 @@
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="E19">
+        <v>0.44915407550050601</v>
+      </c>
+      <c r="F19">
+        <v>5.8639314405256597E-2</v>
+      </c>
+      <c r="G19">
+        <v>0.160917125821957</v>
+      </c>
+      <c r="H19">
+        <v>6.8605903768892496E-3</v>
+      </c>
+      <c r="I19">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
@@ -792,12 +1058,27 @@
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="E20">
+        <v>0.49440811353158298</v>
+      </c>
+      <c r="F20">
+        <v>1.9215863564957299E-2</v>
+      </c>
+      <c r="G20">
+        <v>0.15707954967221099</v>
+      </c>
+      <c r="H20">
+        <v>1.1078821697093301E-2</v>
+      </c>
+      <c r="I20">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -806,12 +1087,27 @@
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="E21">
+        <v>0.24330352153894699</v>
+      </c>
+      <c r="F21">
+        <v>8.8952395680238106E-2</v>
+      </c>
+      <c r="G21">
+        <v>0.105042242970594</v>
+      </c>
+      <c r="H21">
+        <v>7.4811095642773398E-3</v>
+      </c>
+      <c r="I21">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
@@ -820,12 +1116,27 @@
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="E22">
+        <v>0.60312720028665001</v>
+      </c>
+      <c r="F22">
+        <v>7.0397172771075794E-2</v>
+      </c>
+      <c r="G22">
+        <v>0.14413290642589599</v>
+      </c>
+      <c r="H22">
+        <v>1.09797461765874E-2</v>
+      </c>
+      <c r="I22">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B23" t="s">
         <v>12</v>
@@ -834,12 +1145,27 @@
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="E23">
+        <v>0.56801888134600598</v>
+      </c>
+      <c r="F23">
+        <v>6.8305563823099297E-2</v>
+      </c>
+      <c r="G23">
+        <v>0.15016544545015401</v>
+      </c>
+      <c r="H23">
+        <v>9.5147272023419893E-3</v>
+      </c>
+      <c r="I23">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B24" t="s">
         <v>13</v>
@@ -848,12 +1174,27 @@
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="E24">
+        <v>0.49748670972150499</v>
+      </c>
+      <c r="F24">
+        <v>7.1284815048949596E-2</v>
+      </c>
+      <c r="G24">
+        <v>0.16324520110674301</v>
+      </c>
+      <c r="H24">
+        <v>1.19939778091661E-2</v>
+      </c>
+      <c r="I24">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
         <v>14</v>
@@ -862,12 +1203,27 @@
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="E25">
+        <v>0.66505114312490698</v>
+      </c>
+      <c r="F25">
+        <v>6.8045127436781302E-2</v>
+      </c>
+      <c r="G25">
+        <v>0.134929319114863</v>
+      </c>
+      <c r="H25">
+        <v>1.8085032311688301E-2</v>
+      </c>
+      <c r="I25">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B26" t="s">
         <v>6</v>
@@ -876,12 +1232,27 @@
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="E26">
+        <v>0.670471048052797</v>
+      </c>
+      <c r="F26">
+        <v>0.121993651782955</v>
+      </c>
+      <c r="G26">
+        <v>3.4765265407375701</v>
+      </c>
+      <c r="H26">
+        <v>0.36124051897141002</v>
+      </c>
+      <c r="I26">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -890,12 +1261,27 @@
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="E27">
+        <v>0.67851488117317404</v>
+      </c>
+      <c r="F27">
+        <v>0.103878976457424</v>
+      </c>
+      <c r="G27">
+        <v>3.4600615919384401</v>
+      </c>
+      <c r="H27">
+        <v>0.30204000074778298</v>
+      </c>
+      <c r="I27">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
@@ -904,12 +1290,27 @@
         <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="E28">
+        <v>0.66916540923390799</v>
+      </c>
+      <c r="F28">
+        <v>0.108926623748708</v>
+      </c>
+      <c r="G28">
+        <v>3.4777249498290201</v>
+      </c>
+      <c r="H28">
+        <v>0.32616179422699398</v>
+      </c>
+      <c r="I28">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -918,12 +1319,27 @@
         <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="E29">
+        <v>0.51717441990121504</v>
+      </c>
+      <c r="F29">
+        <v>0.10147615840066999</v>
+      </c>
+      <c r="G29">
+        <v>4.0391836501367298</v>
+      </c>
+      <c r="H29">
+        <v>0.366911495560239</v>
+      </c>
+      <c r="I29">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B30" t="s">
         <v>11</v>
@@ -932,12 +1348,27 @@
         <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="E30">
+        <v>0.67840916893386105</v>
+      </c>
+      <c r="F30">
+        <v>5.5900165122333298E-2</v>
+      </c>
+      <c r="G30">
+        <v>3.4518248306185502</v>
+      </c>
+      <c r="H30">
+        <v>0.36954722972149601</v>
+      </c>
+      <c r="I30">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B31" t="s">
         <v>12</v>
@@ -946,12 +1377,27 @@
         <v>9</v>
       </c>
       <c r="D31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="E31">
+        <v>0.73049059052056298</v>
+      </c>
+      <c r="F31">
+        <v>0.121827310352752</v>
+      </c>
+      <c r="G31">
+        <v>3.1526698649301701</v>
+      </c>
+      <c r="H31">
+        <v>0.476043142701774</v>
+      </c>
+      <c r="I31">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B32" t="s">
         <v>13</v>
@@ -960,12 +1406,27 @@
         <v>9</v>
       </c>
       <c r="D32" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="E32">
+        <v>0.68983078034715795</v>
+      </c>
+      <c r="F32">
+        <v>0.12686975624656599</v>
+      </c>
+      <c r="G32">
+        <v>3.4071761552282398</v>
+      </c>
+      <c r="H32">
+        <v>0.48481657974481202</v>
+      </c>
+      <c r="I32">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B33" t="s">
         <v>14</v>
@@ -974,122 +1435,137 @@
         <v>9</v>
       </c>
       <c r="D33" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="E33">
+        <v>0.79059769160848303</v>
+      </c>
+      <c r="F33">
+        <v>6.1251009942600597E-2</v>
+      </c>
+      <c r="G33">
+        <v>2.8585095386283998</v>
+      </c>
+      <c r="H33">
+        <v>0.38851418123896703</v>
+      </c>
+      <c r="I33">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B34" t="s">
         <v>6</v>
       </c>
       <c r="C34" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D34" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B35" t="s">
         <v>7</v>
       </c>
       <c r="C35" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D35" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B36" t="s">
         <v>8</v>
       </c>
       <c r="C36" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D36" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B37" t="s">
         <v>10</v>
       </c>
       <c r="C37" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D37" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B38" t="s">
         <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D38" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B39" t="s">
         <v>12</v>
       </c>
       <c r="C39" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D39" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B40" t="s">
         <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D40" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B41" t="s">
         <v>14</v>
       </c>
       <c r="C41" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D41" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>5</v>
       </c>
@@ -1100,10 +1576,10 @@
         <v>20</v>
       </c>
       <c r="D42" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -1114,10 +1590,10 @@
         <v>20</v>
       </c>
       <c r="D43" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -1128,10 +1604,10 @@
         <v>20</v>
       </c>
       <c r="D44" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>5</v>
       </c>
@@ -1142,10 +1618,10 @@
         <v>20</v>
       </c>
       <c r="D45" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>5</v>
       </c>
@@ -1156,10 +1632,10 @@
         <v>20</v>
       </c>
       <c r="D46" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -1170,10 +1646,10 @@
         <v>20</v>
       </c>
       <c r="D47" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>5</v>
       </c>
@@ -1184,7 +1660,7 @@
         <v>20</v>
       </c>
       <c r="D48" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1198,12 +1674,12 @@
         <v>20</v>
       </c>
       <c r="D49" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B50" t="s">
         <v>6</v>
@@ -1212,12 +1688,12 @@
         <v>20</v>
       </c>
       <c r="D50" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B51" t="s">
         <v>7</v>
@@ -1226,12 +1702,12 @@
         <v>20</v>
       </c>
       <c r="D51" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B52" t="s">
         <v>8</v>
@@ -1240,12 +1716,12 @@
         <v>20</v>
       </c>
       <c r="D52" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B53" t="s">
         <v>10</v>
@@ -1254,12 +1730,12 @@
         <v>20</v>
       </c>
       <c r="D53" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B54" t="s">
         <v>11</v>
@@ -1268,12 +1744,12 @@
         <v>20</v>
       </c>
       <c r="D54" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B55" t="s">
         <v>12</v>
@@ -1282,12 +1758,12 @@
         <v>20</v>
       </c>
       <c r="D55" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B56" t="s">
         <v>13</v>
@@ -1296,12 +1772,12 @@
         <v>20</v>
       </c>
       <c r="D56" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B57" t="s">
         <v>14</v>
@@ -1310,12 +1786,12 @@
         <v>20</v>
       </c>
       <c r="D57" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B58" t="s">
         <v>6</v>
@@ -1324,12 +1800,12 @@
         <v>20</v>
       </c>
       <c r="D58" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B59" t="s">
         <v>7</v>
@@ -1338,12 +1814,12 @@
         <v>20</v>
       </c>
       <c r="D59" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B60" t="s">
         <v>8</v>
@@ -1352,12 +1828,12 @@
         <v>20</v>
       </c>
       <c r="D60" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B61" t="s">
         <v>10</v>
@@ -1366,12 +1842,12 @@
         <v>20</v>
       </c>
       <c r="D61" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B62" t="s">
         <v>11</v>
@@ -1380,12 +1856,12 @@
         <v>20</v>
       </c>
       <c r="D62" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B63" t="s">
         <v>12</v>
@@ -1394,12 +1870,12 @@
         <v>20</v>
       </c>
       <c r="D63" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B64" t="s">
         <v>13</v>
@@ -1408,12 +1884,12 @@
         <v>20</v>
       </c>
       <c r="D64" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B65" t="s">
         <v>14</v>
@@ -1422,1478 +1898,1478 @@
         <v>20</v>
       </c>
       <c r="D65" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B66" t="s">
         <v>6</v>
       </c>
       <c r="C66" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D66" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B67" t="s">
         <v>7</v>
       </c>
       <c r="C67" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D67" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B68" t="s">
         <v>8</v>
       </c>
       <c r="C68" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D68" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B69" t="s">
         <v>10</v>
       </c>
       <c r="C69" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D69" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B70" t="s">
         <v>11</v>
       </c>
       <c r="C70" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D70" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B71" t="s">
         <v>12</v>
       </c>
       <c r="C71" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D71" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B72" t="s">
         <v>13</v>
       </c>
       <c r="C72" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D72" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B73" t="s">
         <v>14</v>
       </c>
       <c r="C73" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D73" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B74" t="s">
         <v>6</v>
       </c>
       <c r="C74" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D74" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B75" t="s">
         <v>7</v>
       </c>
       <c r="C75" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D75" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B76" t="s">
         <v>8</v>
       </c>
       <c r="C76" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D76" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B77" t="s">
         <v>10</v>
       </c>
       <c r="C77" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D77" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B78" t="s">
         <v>11</v>
       </c>
       <c r="C78" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D78" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B79" t="s">
         <v>12</v>
       </c>
       <c r="C79" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D79" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B80" t="s">
         <v>13</v>
       </c>
       <c r="C80" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D80" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B81" t="s">
         <v>14</v>
       </c>
       <c r="C81" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D81" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B82" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C82" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D82" t="s">
-        <v>27</v>
-      </c>
-      <c r="E82">
-        <v>0.57151769551245801</v>
-      </c>
-      <c r="F82">
-        <v>5.7506183115115801E-2</v>
-      </c>
-      <c r="G82">
-        <v>2.5548235393130398</v>
-      </c>
-      <c r="H82">
-        <v>0.125701579706191</v>
-      </c>
-      <c r="I82">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B83" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C83" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D83" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B84" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="C84" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D84" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>17</v>
       </c>
       <c r="B85" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="C85" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D85" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
+        <v>17</v>
+      </c>
+      <c r="B86" t="s">
+        <v>11</v>
+      </c>
+      <c r="C86" t="s">
+        <v>9</v>
+      </c>
+      <c r="D86" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>17</v>
+      </c>
+      <c r="B87" t="s">
+        <v>12</v>
+      </c>
+      <c r="C87" t="s">
+        <v>9</v>
+      </c>
+      <c r="D87" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>17</v>
+      </c>
+      <c r="B88" t="s">
+        <v>13</v>
+      </c>
+      <c r="C88" t="s">
+        <v>9</v>
+      </c>
+      <c r="D88" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>17</v>
+      </c>
+      <c r="B89" t="s">
+        <v>14</v>
+      </c>
+      <c r="C89" t="s">
+        <v>9</v>
+      </c>
+      <c r="D89" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
         <v>18</v>
       </c>
-      <c r="B86" t="s">
-        <v>29</v>
-      </c>
-      <c r="C86" t="s">
-        <v>28</v>
-      </c>
-      <c r="D86" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>5</v>
-      </c>
-      <c r="B87" t="s">
+      <c r="B90" t="s">
         <v>6</v>
       </c>
-      <c r="C87" t="s">
-        <v>21</v>
-      </c>
-      <c r="D87" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>5</v>
-      </c>
-      <c r="B88" t="s">
+      <c r="C90" t="s">
+        <v>9</v>
+      </c>
+      <c r="D90" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>18</v>
+      </c>
+      <c r="B91" t="s">
         <v>7</v>
       </c>
-      <c r="C88" t="s">
-        <v>21</v>
-      </c>
-      <c r="D88" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>5</v>
-      </c>
-      <c r="B89" t="s">
+      <c r="C91" t="s">
+        <v>9</v>
+      </c>
+      <c r="D91" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>18</v>
+      </c>
+      <c r="B92" t="s">
         <v>8</v>
       </c>
-      <c r="C89" t="s">
-        <v>21</v>
-      </c>
-      <c r="D89" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>5</v>
-      </c>
-      <c r="B90" t="s">
+      <c r="C92" t="s">
+        <v>9</v>
+      </c>
+      <c r="D92" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>18</v>
+      </c>
+      <c r="B93" t="s">
         <v>10</v>
       </c>
-      <c r="C90" t="s">
-        <v>21</v>
-      </c>
-      <c r="D90" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>5</v>
-      </c>
-      <c r="B91" t="s">
+      <c r="C93" t="s">
+        <v>9</v>
+      </c>
+      <c r="D93" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>18</v>
+      </c>
+      <c r="B94" t="s">
         <v>11</v>
       </c>
-      <c r="C91" t="s">
-        <v>21</v>
-      </c>
-      <c r="D91" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>5</v>
-      </c>
-      <c r="B92" t="s">
+      <c r="C94" t="s">
+        <v>9</v>
+      </c>
+      <c r="D94" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>18</v>
+      </c>
+      <c r="B95" t="s">
         <v>12</v>
       </c>
-      <c r="C92" t="s">
-        <v>21</v>
-      </c>
-      <c r="D92" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>5</v>
-      </c>
-      <c r="B93" t="s">
+      <c r="C95" t="s">
+        <v>9</v>
+      </c>
+      <c r="D95" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>18</v>
+      </c>
+      <c r="B96" t="s">
         <v>13</v>
       </c>
-      <c r="C93" t="s">
-        <v>21</v>
-      </c>
-      <c r="D93" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>5</v>
-      </c>
-      <c r="B94" t="s">
-        <v>14</v>
-      </c>
-      <c r="C94" t="s">
-        <v>21</v>
-      </c>
-      <c r="D94" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>15</v>
-      </c>
-      <c r="B95" t="s">
-        <v>6</v>
-      </c>
-      <c r="C95" t="s">
-        <v>21</v>
-      </c>
-      <c r="D95" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
-        <v>15</v>
-      </c>
-      <c r="B96" t="s">
-        <v>7</v>
-      </c>
       <c r="C96" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D96" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B97" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C97" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D97" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B98" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C98" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D98" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B99" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C99" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D99" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B100" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C100" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D100" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B101" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C101" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D101" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B102" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C102" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D102" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B103" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C103" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D103" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B104" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C104" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D104" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B105" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C105" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D105" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B106" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C106" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D106" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B107" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C107" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D107" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B108" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C108" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D108" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B109" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C109" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D109" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B110" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C110" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D110" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B111" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C111" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D111" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B112" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C112" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D112" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B113" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C113" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D113" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B114" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C114" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D114" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B115" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C115" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D115" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B116" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C116" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D116" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B117" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C117" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D117" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B118" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C118" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D118" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B119" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C119" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D119" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B120" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C120" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D120" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B121" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C121" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D121" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B122" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C122" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D122" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B123" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C123" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D123" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B124" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C124" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D124" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B125" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C125" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D125" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B126" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C126" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D126" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B127" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C127" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D127" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B128" t="s">
+        <v>13</v>
+      </c>
+      <c r="C128" t="s">
+        <v>20</v>
+      </c>
+      <c r="D128" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>17</v>
+      </c>
+      <c r="B129" t="s">
+        <v>14</v>
+      </c>
+      <c r="C129" t="s">
+        <v>20</v>
+      </c>
+      <c r="D129" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>18</v>
+      </c>
+      <c r="B130" t="s">
+        <v>6</v>
+      </c>
+      <c r="C130" t="s">
+        <v>20</v>
+      </c>
+      <c r="D130" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>18</v>
+      </c>
+      <c r="B131" t="s">
         <v>7</v>
       </c>
-      <c r="C128" t="s">
-        <v>25</v>
-      </c>
-      <c r="D128" t="s">
+      <c r="C131" t="s">
+        <v>20</v>
+      </c>
+      <c r="D131" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>18</v>
+      </c>
+      <c r="B132" t="s">
+        <v>8</v>
+      </c>
+      <c r="C132" t="s">
+        <v>20</v>
+      </c>
+      <c r="D132" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>18</v>
+      </c>
+      <c r="B133" t="s">
+        <v>10</v>
+      </c>
+      <c r="C133" t="s">
+        <v>20</v>
+      </c>
+      <c r="D133" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>18</v>
+      </c>
+      <c r="B134" t="s">
+        <v>11</v>
+      </c>
+      <c r="C134" t="s">
+        <v>20</v>
+      </c>
+      <c r="D134" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>18</v>
+      </c>
+      <c r="B135" t="s">
+        <v>12</v>
+      </c>
+      <c r="C135" t="s">
+        <v>20</v>
+      </c>
+      <c r="D135" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>18</v>
+      </c>
+      <c r="B136" t="s">
+        <v>13</v>
+      </c>
+      <c r="C136" t="s">
+        <v>20</v>
+      </c>
+      <c r="D136" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>18</v>
+      </c>
+      <c r="B137" t="s">
+        <v>14</v>
+      </c>
+      <c r="C137" t="s">
+        <v>20</v>
+      </c>
+      <c r="D137" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>5</v>
+      </c>
+      <c r="B138" t="s">
+        <v>28</v>
+      </c>
+      <c r="C138" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A129" t="s">
-        <v>5</v>
-      </c>
-      <c r="B129" t="s">
-        <v>8</v>
-      </c>
-      <c r="C129" t="s">
-        <v>25</v>
-      </c>
-      <c r="D129" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A130" t="s">
-        <v>5</v>
-      </c>
-      <c r="B130" t="s">
-        <v>10</v>
-      </c>
-      <c r="C130" t="s">
-        <v>25</v>
-      </c>
-      <c r="D130" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
-        <v>5</v>
-      </c>
-      <c r="B131" t="s">
-        <v>11</v>
-      </c>
-      <c r="C131" t="s">
-        <v>25</v>
-      </c>
-      <c r="D131" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
-        <v>5</v>
-      </c>
-      <c r="B132" t="s">
-        <v>12</v>
-      </c>
-      <c r="C132" t="s">
-        <v>25</v>
-      </c>
-      <c r="D132" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A133" t="s">
-        <v>5</v>
-      </c>
-      <c r="B133" t="s">
-        <v>13</v>
-      </c>
-      <c r="C133" t="s">
-        <v>25</v>
-      </c>
-      <c r="D133" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A134" t="s">
-        <v>5</v>
-      </c>
-      <c r="B134" t="s">
-        <v>14</v>
-      </c>
-      <c r="C134" t="s">
-        <v>25</v>
-      </c>
-      <c r="D134" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A135" t="s">
-        <v>15</v>
-      </c>
-      <c r="B135" t="s">
-        <v>6</v>
-      </c>
-      <c r="C135" t="s">
-        <v>25</v>
-      </c>
-      <c r="D135" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A136" t="s">
-        <v>15</v>
-      </c>
-      <c r="B136" t="s">
-        <v>7</v>
-      </c>
-      <c r="C136" t="s">
-        <v>25</v>
-      </c>
-      <c r="D136" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A137" t="s">
-        <v>15</v>
-      </c>
-      <c r="B137" t="s">
-        <v>8</v>
-      </c>
-      <c r="C137" t="s">
-        <v>25</v>
-      </c>
-      <c r="D137" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A138" t="s">
-        <v>15</v>
-      </c>
-      <c r="B138" t="s">
-        <v>10</v>
-      </c>
-      <c r="C138" t="s">
-        <v>25</v>
-      </c>
       <c r="D138" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="E138">
+        <v>0.57151769551245801</v>
+      </c>
+      <c r="F138">
+        <v>5.7506183115115801E-2</v>
+      </c>
+      <c r="G138">
+        <v>2.5548235393130398</v>
+      </c>
+      <c r="H138">
+        <v>0.125701579706191</v>
+      </c>
+      <c r="I138">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>15</v>
       </c>
       <c r="B139" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C139" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D139" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>16</v>
+      </c>
+      <c r="B140" t="s">
+        <v>28</v>
+      </c>
+      <c r="C140" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A140" t="s">
-        <v>15</v>
-      </c>
-      <c r="B140" t="s">
-        <v>12</v>
-      </c>
-      <c r="C140" t="s">
-        <v>25</v>
-      </c>
       <c r="D140" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>17</v>
+      </c>
+      <c r="B141" t="s">
+        <v>28</v>
+      </c>
+      <c r="C141" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A141" t="s">
-        <v>15</v>
-      </c>
-      <c r="B141" t="s">
-        <v>13</v>
-      </c>
-      <c r="C141" t="s">
-        <v>25</v>
-      </c>
       <c r="D141" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>18</v>
+      </c>
+      <c r="B142" t="s">
+        <v>28</v>
+      </c>
+      <c r="C142" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A142" t="s">
-        <v>15</v>
-      </c>
-      <c r="B142" t="s">
-        <v>14</v>
-      </c>
-      <c r="C142" t="s">
-        <v>25</v>
-      </c>
       <c r="D142" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B143" t="s">
         <v>6</v>
       </c>
       <c r="C143" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D143" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B144" t="s">
         <v>7</v>
       </c>
       <c r="C144" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D144" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B145" t="s">
         <v>8</v>
       </c>
       <c r="C145" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D145" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B146" t="s">
         <v>10</v>
       </c>
       <c r="C146" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D146" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B147" t="s">
         <v>11</v>
       </c>
       <c r="C147" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D147" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B148" t="s">
         <v>12</v>
       </c>
       <c r="C148" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D148" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B149" t="s">
         <v>13</v>
       </c>
       <c r="C149" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D149" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B150" t="s">
         <v>14</v>
       </c>
       <c r="C150" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D150" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B151" t="s">
         <v>6</v>
       </c>
       <c r="C151" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D151" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B152" t="s">
         <v>7</v>
       </c>
       <c r="C152" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D152" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B153" t="s">
         <v>8</v>
       </c>
       <c r="C153" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D153" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B154" t="s">
         <v>10</v>
       </c>
       <c r="C154" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D154" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B155" t="s">
         <v>11</v>
       </c>
       <c r="C155" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D155" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B156" t="s">
         <v>12</v>
       </c>
       <c r="C156" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D156" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B157" t="s">
         <v>13</v>
       </c>
       <c r="C157" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D157" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B158" t="s">
         <v>14</v>
       </c>
       <c r="C158" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D158" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B159" t="s">
         <v>6</v>
       </c>
       <c r="C159" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D159" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B160" t="s">
         <v>7</v>
       </c>
       <c r="C160" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D160" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B161" t="s">
         <v>8</v>
       </c>
       <c r="C161" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D161" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B162" t="s">
         <v>10</v>
       </c>
       <c r="C162" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D162" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B163" t="s">
         <v>11</v>
       </c>
       <c r="C163" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D163" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B164" t="s">
         <v>12</v>
       </c>
       <c r="C164" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D164" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B165" t="s">
         <v>13</v>
       </c>
       <c r="C165" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D165" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B166" t="s">
         <v>14</v>
       </c>
       <c r="C166" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D166" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B167" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C167" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D167" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B168" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C168" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D168" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B169" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="C169" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D169" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
@@ -2901,83 +3377,83 @@
         <v>17</v>
       </c>
       <c r="B170" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="C170" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D170" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B171" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C171" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D171" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B172" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C172" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D172" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B173" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C173" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D173" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B174" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C174" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D174" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B175" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C175" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D175" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
@@ -2985,69 +3461,69 @@
         <v>18</v>
       </c>
       <c r="B176" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C176" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D176" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B177" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="C177" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D177" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B178" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="C178" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D178" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B179" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C179" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D179" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B180" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C180" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D180" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
@@ -3055,40 +3531,801 @@
         <v>18</v>
       </c>
       <c r="B181" t="s">
+        <v>13</v>
+      </c>
+      <c r="C181" t="s">
+        <v>21</v>
+      </c>
+      <c r="D181" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>18</v>
+      </c>
+      <c r="B182" t="s">
+        <v>14</v>
+      </c>
+      <c r="C182" t="s">
+        <v>21</v>
+      </c>
+      <c r="D182" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>5</v>
+      </c>
+      <c r="B183" t="s">
+        <v>6</v>
+      </c>
+      <c r="C183" t="s">
+        <v>24</v>
+      </c>
+      <c r="D183" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>5</v>
+      </c>
+      <c r="B184" t="s">
+        <v>7</v>
+      </c>
+      <c r="C184" t="s">
+        <v>24</v>
+      </c>
+      <c r="D184" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>5</v>
+      </c>
+      <c r="B185" t="s">
+        <v>8</v>
+      </c>
+      <c r="C185" t="s">
+        <v>24</v>
+      </c>
+      <c r="D185" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>5</v>
+      </c>
+      <c r="B186" t="s">
+        <v>10</v>
+      </c>
+      <c r="C186" t="s">
+        <v>24</v>
+      </c>
+      <c r="D186" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>5</v>
+      </c>
+      <c r="B187" t="s">
+        <v>11</v>
+      </c>
+      <c r="C187" t="s">
+        <v>24</v>
+      </c>
+      <c r="D187" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>5</v>
+      </c>
+      <c r="B188" t="s">
+        <v>12</v>
+      </c>
+      <c r="C188" t="s">
+        <v>24</v>
+      </c>
+      <c r="D188" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>5</v>
+      </c>
+      <c r="B189" t="s">
+        <v>13</v>
+      </c>
+      <c r="C189" t="s">
+        <v>24</v>
+      </c>
+      <c r="D189" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>5</v>
+      </c>
+      <c r="B190" t="s">
+        <v>14</v>
+      </c>
+      <c r="C190" t="s">
+        <v>24</v>
+      </c>
+      <c r="D190" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>15</v>
+      </c>
+      <c r="B191" t="s">
+        <v>6</v>
+      </c>
+      <c r="C191" t="s">
+        <v>24</v>
+      </c>
+      <c r="D191" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>15</v>
+      </c>
+      <c r="B192" t="s">
+        <v>7</v>
+      </c>
+      <c r="C192" t="s">
+        <v>24</v>
+      </c>
+      <c r="D192" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>15</v>
+      </c>
+      <c r="B193" t="s">
+        <v>8</v>
+      </c>
+      <c r="C193" t="s">
+        <v>24</v>
+      </c>
+      <c r="D193" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>15</v>
+      </c>
+      <c r="B194" t="s">
+        <v>10</v>
+      </c>
+      <c r="C194" t="s">
+        <v>24</v>
+      </c>
+      <c r="D194" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>15</v>
+      </c>
+      <c r="B195" t="s">
+        <v>11</v>
+      </c>
+      <c r="C195" t="s">
+        <v>24</v>
+      </c>
+      <c r="D195" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>15</v>
+      </c>
+      <c r="B196" t="s">
+        <v>12</v>
+      </c>
+      <c r="C196" t="s">
+        <v>24</v>
+      </c>
+      <c r="D196" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>15</v>
+      </c>
+      <c r="B197" t="s">
+        <v>13</v>
+      </c>
+      <c r="C197" t="s">
+        <v>24</v>
+      </c>
+      <c r="D197" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>15</v>
+      </c>
+      <c r="B198" t="s">
+        <v>14</v>
+      </c>
+      <c r="C198" t="s">
+        <v>24</v>
+      </c>
+      <c r="D198" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>16</v>
+      </c>
+      <c r="B199" t="s">
+        <v>6</v>
+      </c>
+      <c r="C199" t="s">
+        <v>24</v>
+      </c>
+      <c r="D199" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>16</v>
+      </c>
+      <c r="B200" t="s">
+        <v>7</v>
+      </c>
+      <c r="C200" t="s">
+        <v>24</v>
+      </c>
+      <c r="D200" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>16</v>
+      </c>
+      <c r="B201" t="s">
+        <v>8</v>
+      </c>
+      <c r="C201" t="s">
+        <v>24</v>
+      </c>
+      <c r="D201" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>16</v>
+      </c>
+      <c r="B202" t="s">
+        <v>10</v>
+      </c>
+      <c r="C202" t="s">
+        <v>24</v>
+      </c>
+      <c r="D202" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>16</v>
+      </c>
+      <c r="B203" t="s">
+        <v>11</v>
+      </c>
+      <c r="C203" t="s">
+        <v>24</v>
+      </c>
+      <c r="D203" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>16</v>
+      </c>
+      <c r="B204" t="s">
+        <v>12</v>
+      </c>
+      <c r="C204" t="s">
+        <v>24</v>
+      </c>
+      <c r="D204" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>16</v>
+      </c>
+      <c r="B205" t="s">
+        <v>13</v>
+      </c>
+      <c r="C205" t="s">
+        <v>24</v>
+      </c>
+      <c r="D205" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>16</v>
+      </c>
+      <c r="B206" t="s">
+        <v>14</v>
+      </c>
+      <c r="C206" t="s">
+        <v>24</v>
+      </c>
+      <c r="D206" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>17</v>
+      </c>
+      <c r="B207" t="s">
+        <v>6</v>
+      </c>
+      <c r="C207" t="s">
+        <v>24</v>
+      </c>
+      <c r="D207" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>17</v>
+      </c>
+      <c r="B208" t="s">
+        <v>7</v>
+      </c>
+      <c r="C208" t="s">
+        <v>24</v>
+      </c>
+      <c r="D208" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
+        <v>17</v>
+      </c>
+      <c r="B209" t="s">
+        <v>8</v>
+      </c>
+      <c r="C209" t="s">
+        <v>24</v>
+      </c>
+      <c r="D209" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>17</v>
+      </c>
+      <c r="B210" t="s">
+        <v>10</v>
+      </c>
+      <c r="C210" t="s">
+        <v>24</v>
+      </c>
+      <c r="D210" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>17</v>
+      </c>
+      <c r="B211" t="s">
+        <v>11</v>
+      </c>
+      <c r="C211" t="s">
+        <v>24</v>
+      </c>
+      <c r="D211" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
+        <v>17</v>
+      </c>
+      <c r="B212" t="s">
+        <v>12</v>
+      </c>
+      <c r="C212" t="s">
+        <v>24</v>
+      </c>
+      <c r="D212" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>17</v>
+      </c>
+      <c r="B213" t="s">
+        <v>13</v>
+      </c>
+      <c r="C213" t="s">
+        <v>24</v>
+      </c>
+      <c r="D213" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>17</v>
+      </c>
+      <c r="B214" t="s">
+        <v>14</v>
+      </c>
+      <c r="C214" t="s">
+        <v>24</v>
+      </c>
+      <c r="D214" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
+        <v>18</v>
+      </c>
+      <c r="B215" t="s">
+        <v>6</v>
+      </c>
+      <c r="C215" t="s">
+        <v>24</v>
+      </c>
+      <c r="D215" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>18</v>
+      </c>
+      <c r="B216" t="s">
+        <v>7</v>
+      </c>
+      <c r="C216" t="s">
+        <v>24</v>
+      </c>
+      <c r="D216" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>18</v>
+      </c>
+      <c r="B217" t="s">
+        <v>8</v>
+      </c>
+      <c r="C217" t="s">
+        <v>24</v>
+      </c>
+      <c r="D217" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>18</v>
+      </c>
+      <c r="B218" t="s">
+        <v>10</v>
+      </c>
+      <c r="C218" t="s">
+        <v>24</v>
+      </c>
+      <c r="D218" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
+        <v>18</v>
+      </c>
+      <c r="B219" t="s">
+        <v>11</v>
+      </c>
+      <c r="C219" t="s">
+        <v>24</v>
+      </c>
+      <c r="D219" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>18</v>
+      </c>
+      <c r="B220" t="s">
+        <v>12</v>
+      </c>
+      <c r="C220" t="s">
+        <v>24</v>
+      </c>
+      <c r="D220" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A221" t="s">
+        <v>18</v>
+      </c>
+      <c r="B221" t="s">
+        <v>13</v>
+      </c>
+      <c r="C221" t="s">
+        <v>24</v>
+      </c>
+      <c r="D221" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A222" t="s">
+        <v>18</v>
+      </c>
+      <c r="B222" t="s">
+        <v>14</v>
+      </c>
+      <c r="C222" t="s">
+        <v>24</v>
+      </c>
+      <c r="D222" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A223" t="s">
+        <v>5</v>
+      </c>
+      <c r="B223" t="s">
+        <v>28</v>
+      </c>
+      <c r="C223" t="s">
+        <v>27</v>
+      </c>
+      <c r="D223" t="s">
         <v>29</v>
       </c>
-      <c r="C181" t="s">
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
+        <v>15</v>
+      </c>
+      <c r="B224" t="s">
         <v>28</v>
       </c>
-      <c r="D181" t="s">
-        <v>32</v>
+      <c r="C224" t="s">
+        <v>27</v>
+      </c>
+      <c r="D224" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
+        <v>16</v>
+      </c>
+      <c r="B225" t="s">
+        <v>28</v>
+      </c>
+      <c r="C225" t="s">
+        <v>27</v>
+      </c>
+      <c r="D225" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
+        <v>17</v>
+      </c>
+      <c r="B226" t="s">
+        <v>28</v>
+      </c>
+      <c r="C226" t="s">
+        <v>27</v>
+      </c>
+      <c r="D226" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
+        <v>18</v>
+      </c>
+      <c r="B227" t="s">
+        <v>28</v>
+      </c>
+      <c r="C227" t="s">
+        <v>27</v>
+      </c>
+      <c r="D227" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
+        <v>5</v>
+      </c>
+      <c r="B228" t="s">
+        <v>28</v>
+      </c>
+      <c r="C228" t="s">
+        <v>27</v>
+      </c>
+      <c r="D228" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A229" t="s">
+        <v>15</v>
+      </c>
+      <c r="B229" t="s">
+        <v>28</v>
+      </c>
+      <c r="C229" t="s">
+        <v>27</v>
+      </c>
+      <c r="D229" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A230" t="s">
+        <v>16</v>
+      </c>
+      <c r="B230" t="s">
+        <v>28</v>
+      </c>
+      <c r="C230" t="s">
+        <v>27</v>
+      </c>
+      <c r="D230" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A231" t="s">
+        <v>17</v>
+      </c>
+      <c r="B231" t="s">
+        <v>28</v>
+      </c>
+      <c r="C231" t="s">
+        <v>27</v>
+      </c>
+      <c r="D231" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
+        <v>18</v>
+      </c>
+      <c r="B232" t="s">
+        <v>28</v>
+      </c>
+      <c r="C232" t="s">
+        <v>27</v>
+      </c>
+      <c r="D232" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A233" t="s">
+        <v>5</v>
+      </c>
+      <c r="B233" t="s">
+        <v>28</v>
+      </c>
+      <c r="C233" t="s">
+        <v>27</v>
+      </c>
+      <c r="D233" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A234" t="s">
+        <v>15</v>
+      </c>
+      <c r="B234" t="s">
+        <v>28</v>
+      </c>
+      <c r="C234" t="s">
+        <v>27</v>
+      </c>
+      <c r="D234" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A235" t="s">
+        <v>16</v>
+      </c>
+      <c r="B235" t="s">
+        <v>28</v>
+      </c>
+      <c r="C235" t="s">
+        <v>27</v>
+      </c>
+      <c r="D235" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A236" t="s">
+        <v>17</v>
+      </c>
+      <c r="B236" t="s">
+        <v>28</v>
+      </c>
+      <c r="C236" t="s">
+        <v>27</v>
+      </c>
+      <c r="D236" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A237" t="s">
+        <v>18</v>
+      </c>
+      <c r="B237" t="s">
+        <v>28</v>
+      </c>
+      <c r="C237" t="s">
+        <v>27</v>
+      </c>
+      <c r="D237" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DDEA578-09EE-4974-A8D3-03AC219B1E2A}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>